<commit_message>
Edited the test files to comply with the new Inventory Template.
BMS-2640
</commit_message>
<xml_diff>
--- a/src/test/resources/Inventory_Import_Template_Bulking.xlsx
+++ b/src/test/resources/Inventory_Import_Template_Bulking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Observation" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ENTRY</t>
   </si>
@@ -44,10 +44,7 @@
     <t>LOCATION</t>
   </si>
   <si>
-    <t>AMOUNT</t>
-  </si>
-  <si>
-    <t>UNITS</t>
+    <t>SEED_AMOUNT_KG</t>
   </si>
   <si>
     <t>COMMENT</t>
@@ -105,7 +102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -133,6 +130,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -189,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,6 +211,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -243,10 +250,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="1:7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -265,7 +272,7 @@
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -293,104 +300,111 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="8" t="n">
+        <v>-753</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7" t="n">
-        <v>-753</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="8" t="n">
+        <v>-754</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="7" t="n">
-        <v>-754</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="8" t="n">
+        <v>-755</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="n">
-        <v>-755</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="8" t="n">
+        <v>-756</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7" t="n">
-        <v>-756</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="n">
+        <v>-757</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="7" t="n">
-        <v>-757</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Modifying files using for tests
Issue: BMS-5101
Reviewer: None
</commit_message>
<xml_diff>
--- a/src/test/resources/Inventory_Import_Template_Bulking.xlsx
+++ b/src/test/resources/Inventory_Import_Template_Bulking.xlsx
@@ -5,94 +5,102 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Observation" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>ENTRY</t>
-  </si>
-  <si>
-    <t>DESIGNATION</t>
-  </si>
-  <si>
-    <t>PARENTAGE</t>
-  </si>
-  <si>
-    <t>GID</t>
-  </si>
-  <si>
-    <t>SOURCE</t>
-  </si>
-  <si>
-    <t>DUPLICATE</t>
-  </si>
-  <si>
-    <t>BULK WITH</t>
-  </si>
-  <si>
-    <t>BULK COMPL?</t>
-  </si>
-  <si>
-    <t>LOCATION</t>
-  </si>
-  <si>
-    <t>SEED_AMOUNT_KG</t>
-  </si>
-  <si>
-    <t>COMMENT</t>
-  </si>
-  <si>
-    <t>MT10A001-1</t>
-  </si>
-  <si>
-    <t>CML502/(CML454 X CML451)-B-3-1-1</t>
-  </si>
-  <si>
-    <t>MT2010F1:1</t>
-  </si>
-  <si>
-    <t>MT10A002-1</t>
-  </si>
-  <si>
-    <t>CLQRCWQ109/(CML454 X CML451)-B-4-1-1</t>
-  </si>
-  <si>
-    <t>MT2010F1:2</t>
-  </si>
-  <si>
-    <t>MT10A003-1</t>
-  </si>
-  <si>
-    <t>CLQRCWQ55/(CML454 X CML451)-B-4-1-2</t>
-  </si>
-  <si>
-    <t>MT2010F1:3</t>
-  </si>
-  <si>
-    <t>MT10A004-1</t>
-  </si>
-  <si>
-    <t>CML165/(CML454 X CML451)-B-4-1-3</t>
-  </si>
-  <si>
-    <t>MT2010F1:4</t>
-  </si>
-  <si>
-    <t>MT10A005-1</t>
-  </si>
-  <si>
-    <t>CLQRCWQ38/(CML454 X CML451)-B-4-2-1</t>
-  </si>
-  <si>
-    <t>MT2010F1:5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <si>
+    <t xml:space="preserve">ENTRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESIGNATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARENTAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOURCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUPLICATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BULK WITH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BULK COMPL?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCATION ABBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEED_AMOUNT_KG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT10A001-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CML502/(CML454 X CML451)-B-3-1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT2010F1:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT10A002-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLQRCWQ109/(CML454 X CML451)-B-4-1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT2010F1:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT10A003-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLQRCWQ55/(CML454 X CML451)-B-4-1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT2010F1:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT10A004-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CML165/(CML454 X CML451)-B-4-1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT2010F1:4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT10A005-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLQRCWQ38/(CML454 X CML451)-B-4-2-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT2010F1:5</t>
   </si>
 </sst>
 </file>
@@ -100,9 +108,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -130,12 +138,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -213,7 +215,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -250,26 +252,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.015306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -300,111 +302,105 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AMJ1" s="0"/>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="8" t="n">
         <v>-753</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AMJ2" s="0"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="3" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="8" t="n">
         <v>-754</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AMJ3" s="0"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="4" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="8" t="n">
         <v>-755</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="AMJ4" s="0"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="5" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="8" t="n">
         <v>-756</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AMJ5" s="0"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>-757</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="I6" s="9"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>